<commit_message>
first working code on gpu machine
</commit_message>
<xml_diff>
--- a/EXCEL_OUPUT/20 MAA -  Financial Report  (Signed).xlsx
+++ b/EXCEL_OUPUT/20 MAA -  Financial Report  (Signed).xlsx
@@ -45,12 +45,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="743">
-  <si>
-    <t>EmErfury</t>
-  </si>
-  <si>
-    <t>Ernst &amp;Young</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="745">
+  <si>
+    <t>Ertryoug</t>
+  </si>
+  <si>
+    <t>Ernst &amp; Young</t>
   </si>
   <si>
     <t>Jacob Gossan</t>
@@ -326,7 +326,7 @@
     <t>(9,032)</t>
   </si>
   <si>
-    <t>facilities</t>
+    <t>Total facilities</t>
   </si>
   <si>
     <t>Utilised</t>
@@ -716,7 +716,7 @@
     <t>1743</t>
   </si>
   <si>
-    <t>Construction inj progress</t>
+    <t>Construction in progress</t>
   </si>
   <si>
     <t>2538</t>
@@ -812,7 +812,10 @@
     <t>54535</t>
   </si>
   <si>
-    <t>At 1 January</t>
+    <t>b)</t>
+  </si>
+  <si>
+    <t>At 1. January</t>
   </si>
   <si>
     <t>Share of gain/(loss) of joint venture, net of tax</t>
@@ -1076,7 +1079,7 @@
     <t>Deferred tax benefit</t>
   </si>
   <si>
-    <t>Net deferred tax assets/liabilities)</t>
+    <t>Net deferred tax assets/(liabilities)</t>
   </si>
   <si>
     <t>Reflected in the statement of financial position</t>
@@ -1091,7 +1094,7 @@
     <t>Deferred tax liabilities</t>
   </si>
   <si>
-    <t>Deferred tax assets/liabilities), net</t>
+    <t>Deferred tax assets/(liabilities), net</t>
   </si>
   <si>
     <t>Statement of profit or loss Statement of financial and other comprehensive position income</t>
@@ -1250,6 +1253,9 @@
     <t>Depreciation</t>
   </si>
   <si>
+    <t>Depreciation -</t>
+  </si>
+  <si>
     <t>Included in administrative expenses:</t>
   </si>
   <si>
@@ -1352,12 +1358,15 @@
     <t>Australia</t>
   </si>
   <si>
-    <t>Timing of revenue recognition</t>
+    <t>Timing of recognition</t>
   </si>
   <si>
     <t>Goods transferred at a point in time</t>
   </si>
   <si>
+    <t>Total from contracts with customers</t>
+  </si>
+  <si>
     <t>4.2 Other revenue</t>
   </si>
   <si>
@@ -1433,10 +1442,10 @@
     <t>Estimation of useful lives of assets</t>
   </si>
   <si>
-    <t>The estimation of useful lives is based on historical experience as well as</t>
-  </si>
-  <si>
-    <t>of the period over</t>
+    <t>The estimation of useful lives is based on historical</t>
+  </si>
+  <si>
+    <t>oft the period over</t>
   </si>
   <si>
     <t>annually by the</t>
@@ -1487,7 +1496,7 @@
     <t>The Company</t>
   </si>
   <si>
-    <t>covered by an option to extend the lease if it is</t>
+    <t>covered by an option to extend the lease if it is reasonably certain to be exercised, or any periods covered by an</t>
   </si>
   <si>
     <t>option to terminate</t>
@@ -1505,7 +1514,7 @@
     <t>exercise the renewal option, or not exercise the</t>
   </si>
   <si>
-    <t>reassesses the lease term if there is a significant</t>
+    <t>the lease term if there is a significant</t>
   </si>
   <si>
     <t>affects its ability strategy).</t>
@@ -1532,6 +1541,9 @@
     <t>to exercise (or not to exercise)</t>
   </si>
   <si>
+    <t>experience as well as</t>
+  </si>
+  <si>
     <t>expectation of future events.</t>
   </si>
   <si>
@@ -1547,9 +1559,6 @@
     <t>non-cancellable term of the lease, together with</t>
   </si>
   <si>
-    <t>reasonably certain to be exercised, or any periods covered by an</t>
-  </si>
-  <si>
     <t>exercised, or the termination option will not be exercised. That</t>
   </si>
   <si>
@@ -1619,7 +1628,7 @@
     <t>Any differences between the amounts receivable or payable under the tax funding agreement are recognised as</t>
   </si>
   <si>
-    <t>a contribution to (or distribution from) wholly-owned tax consolidated entities.</t>
+    <t>acontribution to (or distribution from) wholly-owned tax consolidated entities.</t>
   </si>
   <si>
     <t>Goods and services tax (GST)</t>
@@ -1631,7 +1640,7 @@
     <t>When the GST</t>
   </si>
   <si>
-    <t>the taxation authority, in which case the GST is recognised as part of the revenue or the expense item</t>
+    <t>the taxation authority, in which case the GST is recognised as part of the revenue or the expense item or</t>
   </si>
   <si>
     <t>as part of the cost of acquisition of the asset, as applicable</t>
@@ -1679,7 +1688,7 @@
     <t>comparative figures have been reclassified to conform with changes</t>
   </si>
   <si>
-    <t>recoverable</t>
+    <t>recoverable from</t>
   </si>
   <si>
     <t>as part of receivables</t>
@@ -1700,9 +1709,6 @@
     <t>Buildings</t>
   </si>
   <si>
-    <t>Construction in progress</t>
-  </si>
-  <si>
     <t>Not depreciated</t>
   </si>
   <si>
@@ -1721,7 +1727,7 @@
     <t>The new and amended Australian Accounting Standards and Interpretations that apply for the first time in 2020,</t>
   </si>
   <si>
-    <t>do not materially impact the financial statements of the Company.</t>
+    <t>dor not materially impact the financial statements of the Company.</t>
   </si>
   <si>
     <t>Accounting Standards and Interpretations issued but not yet effective</t>
@@ -1745,7 +1751,7 @@
     <t>a) Current versus non-current classification</t>
   </si>
   <si>
-    <t>The Company presents assets and liabilities in the statement of financial position based on currenthnon-current classification. An asset is current when it is:</t>
+    <t>The Company presents assets and liabilities in the statement of financial position based on current/non-current classification. An asset is current when it is:</t>
   </si>
   <si>
     <t>Expected to be realised or intended to be sold or consumed in the normal operating cycle;</t>
@@ -1766,7 +1772,7 @@
     <t>A liability is current when:</t>
   </si>
   <si>
-    <t>Itis expected to be settled in the normal operating cycle;</t>
+    <t>Itise expected to be settled in the normal operating cycle;</t>
   </si>
   <si>
     <t>Itis held primarily for the purpose of trading;</t>
@@ -1790,7 +1796,7 @@
     <t>Both the functional and presentation currency of the Company is the Australian dollar ($).</t>
   </si>
   <si>
-    <t>Transactions and balances</t>
+    <t>- Transactions and balances</t>
   </si>
   <si>
     <t>Transactions in foreign currencies are initially recorded by the Company's entities at their respective functional currency by applying the exchange rates ruling (either at spot rates, hedge rates, or rates suppliers applied on</t>
@@ -1847,7 +1853,7 @@
     <t>Net cash flows used in financing activities</t>
   </si>
   <si>
-    <t>Net (decrease/increase in cash and cash equivalents</t>
+    <t>Net (decrease )increase in cash and cash equivalents</t>
   </si>
   <si>
     <t>Cash and cash equivalents at beginning of the year</t>
@@ -1928,7 +1934,7 @@
     <t>23777</t>
   </si>
   <si>
-    <t>As at1January! 2020</t>
+    <t>Asa at1January 2020</t>
   </si>
   <si>
     <t>Loss for the year</t>
@@ -1940,7 +1946,7 @@
     <t>Total comprehensive loss for the year</t>
   </si>
   <si>
-    <t>As at1J January 2019</t>
+    <t>Asat1January 2019</t>
   </si>
   <si>
     <t>Other comprehensive (loss)/gain</t>
@@ -1955,13 +1961,13 @@
     <t>Contributed equity (Note 18)</t>
   </si>
   <si>
-    <t>Cash flow hedge reserve (Note 19)</t>
+    <t>Cashflow hedge reserve (Note 19)</t>
   </si>
   <si>
     <t>Reserve in joint venture (Note 19)</t>
   </si>
   <si>
-    <t>Otherreserve (Note 19)</t>
+    <t>Other reserve (Note 19)</t>
   </si>
   <si>
     <t>Accumulated losses</t>
@@ -2234,13 +2240,13 @@
     <t>Other comprehensive loss Other comprehensive loss that will not be reclassified to profit or loss in subsequent periods:</t>
   </si>
   <si>
-    <t>Actuarial (loss) )gains on defined benefit plans</t>
+    <t>Actuarial (loss)/gains on defined benefit plans</t>
   </si>
   <si>
     <t>Income tax effect</t>
   </si>
   <si>
-    <t>Othercomprehensive loss that may be reclassified to profit or loss in subsequent periods:</t>
+    <t>Other comprehensive loss that may be reclassified to profit or loss in subsequent periods:</t>
   </si>
   <si>
     <t>Net movement of cash flow hedges</t>
@@ -2631,44 +2637,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3165,6 +3189,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>255</v>
+      </c>
+    </row>
     <row r="3" spans="1:4">
       <c r="C3" t="s">
         <v>8</v>
@@ -3183,29 +3212,29 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C5" t="s">
         <v>254</v>
       </c>
       <c r="D5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C6" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C7" t="s">
         <v>81</v>
@@ -3216,7 +3245,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C8" t="s">
         <v>253</v>
@@ -3251,7 +3280,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3277,37 +3306,37 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="B9" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C9" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3317,15 +3346,15 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C11" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3346,7 +3375,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B15" t="s">
         <v>253</v>
@@ -3384,7 +3413,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3405,26 +3434,26 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B6" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3445,37 +3474,37 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D10" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C11" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D11" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="C12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D12" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3496,32 +3525,32 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C16" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D16" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C17" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D17" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="C18" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D18" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -3550,7 +3579,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3576,23 +3605,23 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C6" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C7" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="C8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3602,10 +3631,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C10" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -3634,7 +3663,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3655,65 +3684,65 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B5" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C5" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B6" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C6" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C7" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B8" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C9" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B10" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C10" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -3758,46 +3787,46 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B4" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C4" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C5" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B6" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B7" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -3832,16 +3861,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3874,84 +3903,84 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B5" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D5" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C6" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D6" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E6" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B7" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C7" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D7" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E7" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B8" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C8" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D8" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E8" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B9" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C9" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D9" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E9" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -3959,33 +3988,33 @@
         <v>151</v>
       </c>
       <c r="B10" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C10" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D10" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E10" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B11" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C11" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D11" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E11" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -3993,117 +4022,117 @@
         <v>155</v>
       </c>
       <c r="B12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C12" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D12" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E12" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B13" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D13" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="E13" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B14" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D14" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B15" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D15" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D16" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E16" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B17" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C17" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B20" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C20" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B21" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C21" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B22" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C22" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -4212,58 +4241,58 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B5" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C5" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B10" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C10" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -4311,82 +4340,82 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B4" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B5" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C5" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D5" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B6" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C6" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D6" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B7" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B8" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C8" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="D8" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B9" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C9" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="D9" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="C10" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D10" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -4431,18 +4460,18 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B4" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C4" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4463,32 +4492,32 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B8" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C8" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B9" t="s">
         <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="B10" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="C10" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -4517,22 +4546,22 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4553,99 +4582,99 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B9" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="C9" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B10" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="C10" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B12" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="C12" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B13" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="C13" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B14" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="C14" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B16" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="C16" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>431</v>
+        <v>439</v>
       </c>
       <c r="B17" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="C17" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -4666,18 +4695,18 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="B21" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="C21" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -4698,48 +4727,48 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="B25" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="C25" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="C26" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="C27" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B28" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="C28" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="B29" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C29" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -4774,113 +4803,113 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="B2" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="C2" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="D2" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="B3" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="B4" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="B5" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C5" t="s">
-        <v>462</v>
+        <v>498</v>
       </c>
       <c r="D5" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="E5" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="B6" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="C6" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="D6" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="E6" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="B7" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="C7" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="D7" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="B8" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="B9" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="C9" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="D9" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="E9" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="B10" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -4893,300 +4922,300 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="B12" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="C12" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="D12" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="E12" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="B13" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="C13" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="D13" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="B14" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="B15" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="C15" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="D15" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="E15" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="B16" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="C16" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="B17" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="B18" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="C18" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="D18" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="E18" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="B19" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="C19" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="D19" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="E19" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="B20" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="C20" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="D20" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="E20" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="B21" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="C21" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="B22" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="C22" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="D22" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="B23" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="C23" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="D23" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="E23" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="B24" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="C24" t="s">
-        <v>500</v>
+        <v>483</v>
       </c>
       <c r="D24" t="s">
-        <v>500</v>
+        <v>483</v>
       </c>
       <c r="E24" t="s">
-        <v>500</v>
+        <v>483</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="B25" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="C25" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="B26" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="C26" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="D26" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="E26" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="B27" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="C27" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="D27" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="E27" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="B28" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="C28" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="D28" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="E28" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="B29" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="C29" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="D29" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="E29" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="B30" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="C30" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="D30" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="E30" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="B31" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="C31" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="D31" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="E31" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -5218,220 +5247,220 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="B2" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="C2" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="B3" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="C3" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="B4" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="B5" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="C5" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="D5" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="B6" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="C6" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="B7" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="B8" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="C8" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="B9" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="C9" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="D9" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="B10" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="C10" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="D10" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="B11" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="C11" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="B12" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="C12" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="B13" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="C13" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="D13" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="B14" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="C14" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="D14" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="B15" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="C15" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="B16" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="C16" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="D16" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="B17" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="C17" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="D17" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="B18" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="B20" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="C20" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="D20" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>
@@ -5457,18 +5486,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="B2" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="B3" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5476,15 +5505,15 @@
         <v>202</v>
       </c>
       <c r="B4" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>551</v>
+        <v>223</v>
       </c>
       <c r="B5" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
     </row>
   </sheetData>
@@ -5507,167 +5536,167 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
   </sheetData>
@@ -5707,7 +5736,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -5718,193 +5747,193 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="C5" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="D5" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="C6" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="D6" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="C7" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="D7" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="C8" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D8" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="C9" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D9" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C10" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="D10" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="C11" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="D11" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="C13" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="D13" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="C14" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="D14" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="C16" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="D16" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D17" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="C18" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="D18" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="C19" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="D19" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="C20" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="D20" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="C21" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D21" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="B22" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="C22" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -5945,22 +5974,22 @@
     </row>
     <row r="2" spans="1:7">
       <c r="B2" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="C2" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="D2" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="E2" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="F2" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="G2" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -5985,7 +6014,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="B4" t="s">
         <v>144</v>
@@ -6000,26 +6029,26 @@
         <v>83</v>
       </c>
       <c r="F4" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="G4" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="F5" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="G5" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="C6" t="s">
         <v>78</v>
@@ -6031,12 +6060,12 @@
         <v>123</v>
       </c>
       <c r="G6" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="C7" t="s">
         <v>78</v>
@@ -6045,10 +6074,10 @@
         <v>81</v>
       </c>
       <c r="F7" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="G7" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -6068,15 +6097,15 @@
         <v>83</v>
       </c>
       <c r="F8" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="G8" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="B9" t="s">
         <v>144</v>
@@ -6091,26 +6120,26 @@
         <v>83</v>
       </c>
       <c r="F9" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="G9" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="F10" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="G10" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="C11" t="s">
         <v>88</v>
@@ -6119,15 +6148,15 @@
         <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="G11" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="C12" t="s">
         <v>88</v>
@@ -6136,15 +6165,15 @@
         <v>90</v>
       </c>
       <c r="F12" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="G12" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="B13" t="s">
         <v>144</v>
@@ -6159,10 +6188,10 @@
         <v>83</v>
       </c>
       <c r="F13" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="G13" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
     </row>
   </sheetData>
@@ -6393,12 +6422,12 @@
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -6408,55 +6437,55 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="B7" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="C7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B8" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="C8" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D8" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="B9" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="C9" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D9" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B10" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="D10" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -6464,38 +6493,38 @@
         <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="C11" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="D11" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="B12" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C12" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D12" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="C13" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="D13" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -6505,10 +6534,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="B15" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="C15" t="s">
         <v>253</v>
@@ -6519,10 +6548,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B16" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="C16" t="s">
         <v>237</v>
@@ -6533,10 +6562,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B17" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="C17" t="s">
         <v>245</v>
@@ -6547,49 +6576,49 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B18" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="D18" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B19" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="C19" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D19" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="B20" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D20" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="C21" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="D21" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -6597,15 +6626,15 @@
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="D22" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -6626,10 +6655,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="B26" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="D26" t="s">
         <v>102</v>
@@ -6637,24 +6666,24 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B27" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C27" t="s">
         <v>141</v>
       </c>
       <c r="D27" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B28" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="C28" t="s">
         <v>173</v>
@@ -6665,7 +6694,7 @@
         <v>155</v>
       </c>
       <c r="B29" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="C29" t="s">
         <v>158</v>
@@ -6676,13 +6705,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="C30" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="D30" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -6703,16 +6732,16 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B33" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C33" t="s">
         <v>142</v>
       </c>
       <c r="D33" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -6720,7 +6749,7 @@
         <v>155</v>
       </c>
       <c r="B34" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="C34" t="s">
         <v>159</v>
@@ -6731,27 +6760,27 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B35" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="C35" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="D35" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="C36" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="D36" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -6759,10 +6788,10 @@
         <v>21</v>
       </c>
       <c r="C37" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="D37" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -6770,23 +6799,23 @@
         <v>22</v>
       </c>
       <c r="C38" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="D38" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="B40" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C40" t="s">
         <v>144</v>
@@ -6797,21 +6826,21 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="C41" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D41" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="B42" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="C42" t="s">
         <v>86</v>
@@ -6822,13 +6851,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="C43" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="D43" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
     </row>
   </sheetData>
@@ -6860,7 +6889,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6873,7 +6902,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -6884,177 +6913,177 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B5" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="C5" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="D5" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="B6" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="C6" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="D6" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="C7" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="D7" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="C8" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="D8" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="C9" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="D9" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="B10" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C10" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="D10" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B11" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="C11" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="C12" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="D12" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="B13" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="C13" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D13" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="B14" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="C14" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="D14" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="B15" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="C15" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="C16" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D16" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="B17" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="C17" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D17" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="C18" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="D18" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
     </row>
   </sheetData>
@@ -7086,35 +7115,35 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="B2" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B3" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="C3" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="D3" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C4" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="D4" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -7122,37 +7151,37 @@
         <v>123</v>
       </c>
       <c r="D5" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="B6" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="C7" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="D7" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C8" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="D8" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -7165,10 +7194,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B10" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="C10" t="s">
         <v>81</v>
@@ -7179,27 +7208,27 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="B11" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="C11" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="D11" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="C12" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="D12" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
     </row>
   </sheetData>

</xml_diff>